<commit_message>
Corrections règlements spécifique et liste des bourses
</commit_message>
<xml_diff>
--- a/excel/prix.xlsx
+++ b/excel/prix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8544C1B4-92C5-B24E-AA4E-4C4F46C0E9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100C125E-86B3-9E4F-9863-8EF5E5FFD128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="560" windowWidth="33480" windowHeight="20380" activeTab="9" xr2:uid="{CE5E1F58-89A2-BD42-AA5E-6DDAA3F3C6F4}"/>
+    <workbookView xWindow="76820" yWindow="560" windowWidth="25520" windowHeight="28180" activeTab="9" xr2:uid="{CE5E1F58-89A2-BD42-AA5E-6DDAA3F3C6F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Etape" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Total" sheetId="8" r:id="rId9"/>
     <sheet name="Verif_UCI" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>montant</t>
   </si>
@@ -128,15 +128,9 @@
     <t>Min_UCI</t>
   </si>
   <si>
-    <t>Taux de change officiel UCI (https://assets.ctfassets.net/761l7gh5x5an/5G5JfslUY9ynE73LV2g9Zi/83a927bf79ee339a0df921fef64fe385/FX_officiel_UCI_2023_-_Multi.pdf)</t>
-  </si>
-  <si>
     <t>Obligations minimales pour 2023</t>
   </si>
   <si>
-    <t>https://assets.ctfassets.net/761l7gh5x5an/4LhHQ0knlVpQFA1wf3X2Re/d6066b0cb0f95507c1117cf0e1afdb13/ROA-20220420_-_2023_Road_Financial_Obligations_-v2_PW_Lbo_Corrected_17.06.2022.pdf</t>
-  </si>
-  <si>
     <t>Validation se fait en rouge si montant pas assez élevé, dans Onglets Etape, Demi-Étape, GenTemps</t>
   </si>
   <si>
@@ -153,6 +147,15 @@
   </si>
   <si>
     <t>Étapes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taux de change officiel UCI </t>
+  </si>
+  <si>
+    <t>https://assets.ctfassets.net/761l7gh5x5an/5G5JfslUY9ynE73LV2g9Zi/0521c8a2b8950abb454eaabfc819cce3/16.FX_officiel_UCI_2024_-_Multi.pdf</t>
+  </si>
+  <si>
+    <t>https://assets.ctfassets.net/761l7gh5x5an/3XSdDT5GZNHaRDKjjqE4bo/d586af08d8940967b7e4cdac1d14bc18/ROA-20231008_-_2024_Road_Financial_Obligations.pdf</t>
   </si>
 </sst>
 </file>
@@ -299,10 +302,103 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>135816</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1DB30C4-8F82-F071-C894-8DF0A87B81B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="7277100"/>
+          <a:ext cx="7772400" cy="2409116"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>688636</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BC6E13F-31FE-E523-17DC-5CF2C3939DF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9702800" y="317500"/>
+          <a:ext cx="9972336" cy="4191000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -340,7 +436,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -446,7 +542,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -588,7 +684,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,7 +695,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,10 +713,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -628,14 +724,14 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C2">
         <v>175</v>
       </c>
       <c r="D2" s="3">
         <f>ROUNDUP(C2*Verif_UCI!$B$29,0)</f>
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -643,14 +739,14 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
       <c r="D3" s="3">
         <f>ROUNDUP(C3*Verif_UCI!$B$29,0)</f>
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -665,7 +761,7 @@
       </c>
       <c r="D4" s="3">
         <f>ROUNDUP(C4*Verif_UCI!$B$29,0)</f>
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -680,7 +776,7 @@
       </c>
       <c r="D5" s="3">
         <f>ROUNDUP(C5*Verif_UCI!$B$29,0)</f>
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -695,7 +791,7 @@
       </c>
       <c r="D6" s="3">
         <f>ROUNDUP(C6*Verif_UCI!$B$29,0)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -712,7 +808,7 @@
       </c>
       <c r="D7" s="3">
         <f>ROUNDUP(C7*Verif_UCI!$B$29,0)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -729,7 +825,7 @@
       </c>
       <c r="D8" s="3">
         <f>ROUNDUP(C8*Verif_UCI!$B$29,0)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -746,7 +842,7 @@
       </c>
       <c r="D9" s="3">
         <f>ROUNDUP(C9*Verif_UCI!$B$29,0)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -763,7 +859,7 @@
       </c>
       <c r="D10" s="3">
         <f>ROUNDUP(C10*Verif_UCI!$B$29,0)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -780,7 +876,7 @@
       </c>
       <c r="D11" s="3">
         <f>ROUNDUP(C11*Verif_UCI!$B$29,0)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -795,7 +891,7 @@
       </c>
       <c r="D12" s="3">
         <f>ROUNDUP(C12*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -812,7 +908,7 @@
       </c>
       <c r="D13" s="3">
         <f>ROUNDUP(C13*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -829,7 +925,7 @@
       </c>
       <c r="D14" s="3">
         <f>ROUNDUP(C14*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -846,7 +942,7 @@
       </c>
       <c r="D15" s="3">
         <f>ROUNDUP(C15*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -863,7 +959,7 @@
       </c>
       <c r="D16" s="3">
         <f>ROUNDUP(C16*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -880,7 +976,7 @@
       </c>
       <c r="D17" s="3">
         <f>ROUNDUP(C17*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -897,7 +993,7 @@
       </c>
       <c r="D18" s="3">
         <f>ROUNDUP(C18*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -914,7 +1010,7 @@
       </c>
       <c r="D19" s="3">
         <f>ROUNDUP(C19*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -931,7 +1027,7 @@
       </c>
       <c r="D20" s="3">
         <f>ROUNDUP(C20*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -948,7 +1044,7 @@
       </c>
       <c r="D21" s="3">
         <f>ROUNDUP(C21*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -957,7 +1053,7 @@
       </c>
       <c r="B22">
         <f>SUM(B2:B21)</f>
-        <v>1350</v>
+        <v>1360</v>
       </c>
     </row>
   </sheetData>
@@ -976,7 +1072,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1132,7 @@
         <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2">
         <v>0.2</v>
@@ -1048,39 +1144,39 @@
       </c>
       <c r="B3">
         <f>IF(B$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C3">
         <f>IF(C$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D3">
         <f>IF(D$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E3">
         <f>IF(E$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F3">
         <f>IF(F$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="G3">
         <f>IF(G$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="H3">
         <f>IF(H$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I22" si="0">SUM(B3:H3)</f>
-        <v>1565</v>
+        <v>1600</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J22" si="1">I3*$J$2</f>
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1089,11 +1185,11 @@
       </c>
       <c r="B4">
         <f>IF(B$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C4">
         <f>IF(C$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D4">
         <f>IF(D$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
@@ -1105,23 +1201,23 @@
       </c>
       <c r="F4">
         <f>IF(F$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G4">
         <f>IF(G$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="H4">
         <f>IF(H$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>945</v>
+        <v>970</v>
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1865,49 +1961,54 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I24">
         <f>SUM(I3:I22)</f>
-        <v>8670</v>
+        <v>8730</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B29" s="1">
-        <v>1.4487000000000001</v>
+        <v>1.462</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A32" r:id="rId1" xr:uid="{E5D767CF-292E-DC4B-BC13-706ECDC64A88}"/>
+    <hyperlink ref="D28" r:id="rId1" xr:uid="{A34B989D-C56F-EF49-B015-1E596F048139}"/>
+    <hyperlink ref="A32" r:id="rId2" xr:uid="{5FD4F4A4-3B0E-D740-A5C4-717092981AAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1916,7 +2017,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1934,10 +2035,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1945,14 +2046,14 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" s="3">
         <f>ROUNDUP(C2*Verif_UCI!$B$29,0)</f>
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1967,7 +2068,7 @@
       </c>
       <c r="D3" s="3">
         <f>ROUNDUP(C3*Verif_UCI!$B$29,0)</f>
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1982,7 +2083,7 @@
       </c>
       <c r="D4" s="3">
         <f>ROUNDUP(C4*Verif_UCI!$B$29,0)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1997,7 +2098,7 @@
       </c>
       <c r="D5" s="3">
         <f>ROUNDUP(C5*Verif_UCI!$B$29,0)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2112,7 +2213,7 @@
       </c>
       <c r="D12" s="3">
         <f>ROUNDUP(C12*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2129,7 +2230,7 @@
       </c>
       <c r="D13" s="3">
         <f>ROUNDUP(C13*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2146,7 +2247,7 @@
       </c>
       <c r="D14" s="3">
         <f>ROUNDUP(C14*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2163,7 +2264,7 @@
       </c>
       <c r="D15" s="3">
         <f>ROUNDUP(C15*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2180,7 +2281,7 @@
       </c>
       <c r="D16" s="3">
         <f>ROUNDUP(C16*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2197,7 +2298,7 @@
       </c>
       <c r="D17" s="3">
         <f>ROUNDUP(C17*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2214,7 +2315,7 @@
       </c>
       <c r="D18" s="3">
         <f>ROUNDUP(C18*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2231,7 +2332,7 @@
       </c>
       <c r="D19" s="3">
         <f>ROUNDUP(C19*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2248,7 +2349,7 @@
       </c>
       <c r="D20" s="3">
         <f>ROUNDUP(C20*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2265,7 +2366,7 @@
       </c>
       <c r="D21" s="3">
         <f>ROUNDUP(C21*Verif_UCI!$B$29,0)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2274,7 +2375,7 @@
       </c>
       <c r="B22">
         <f>SUM(B2:B21)</f>
-        <v>960</v>
+        <v>965</v>
       </c>
     </row>
   </sheetData>
@@ -2293,7 +2394,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2322,7 +2423,7 @@
       </c>
       <c r="C2">
         <f>Verif_UCI!J3</f>
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2334,7 +2435,7 @@
       </c>
       <c r="C3">
         <f>Verif_UCI!J4</f>
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2563,14 +2664,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C221">
-    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="greaterThan">
-      <formula>$B$2</formula>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>B2-C2 &lt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B21">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>B2-C2 &lt;0</formula>
+  <conditionalFormatting sqref="C2:C221">
+    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="greaterThan">
+      <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2583,7 +2684,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2604,7 +2705,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2629,7 +2730,7 @@
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2643,7 +2744,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2664,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2689,7 +2790,7 @@
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2703,7 +2804,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2724,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2749,7 +2850,7 @@
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2763,7 +2864,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2792,7 +2893,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2800,7 +2901,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2809,7 +2910,7 @@
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -2908,14 +3009,14 @@
       </c>
       <c r="B3">
         <f>GenPoints!B5</f>
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2924,14 +3025,14 @@
       </c>
       <c r="B4">
         <f>GenEquipe!B5</f>
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2940,14 +3041,14 @@
       </c>
       <c r="B5">
         <f>GenKOM!B5</f>
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2956,14 +3057,14 @@
       </c>
       <c r="B6">
         <f>GenJeune!B5</f>
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2988,14 +3089,14 @@
       </c>
       <c r="B8">
         <f>Etape!B22</f>
-        <v>1350</v>
+        <v>1360</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>6750</v>
+        <v>6800</v>
       </c>
       <c r="E8" s="5"/>
     </row>
@@ -3005,14 +3106,14 @@
       </c>
       <c r="B9">
         <f>DemiEtape!B22</f>
-        <v>960</v>
+        <v>965</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1920</v>
+        <v>1930</v>
       </c>
       <c r="E9" s="5"/>
     </row>
@@ -3022,7 +3123,7 @@
       </c>
       <c r="D10" s="1">
         <f>SUM(D2:D9)</f>
-        <v>11725</v>
+        <v>11815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>